<commit_message>
update code auth and registerExecuteCapstone, sigin
</commit_message>
<xml_diff>
--- a/server/files/users.xlsx
+++ b/server/files/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>S no.</t>
   </si>
@@ -34,10 +34,16 @@
     <t>Department Code</t>
   </si>
   <si>
-    <t>Department Name</t>
+    <t>Department</t>
   </si>
   <si>
     <t>cnnguyenvantien@gmail.com</t>
+  </si>
+  <si>
+    <t>CMU</t>
+  </si>
+  <si>
+    <t>Khoa đào tạo quốc tế</t>
   </si>
   <si>
     <t/>
@@ -474,48 +480,72 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -523,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
submit, upadate topic template function
</commit_message>
<xml_diff>
--- a/server/files/users.xlsx
+++ b/server/files/users.xlsx
@@ -4,86 +4,47 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="My Users" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Capstone 2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
-  <si>
-    <t>S no.</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Academic Level</t>
-  </si>
-  <si>
-    <t>Department Code</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>cnnguyenvantien@gmail.com</t>
-  </si>
-  <si>
-    <t>CMU</t>
-  </si>
-  <si>
-    <t>Khoa đào tạo quốc tế</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>hoctap432000@gmail.com</t>
-  </si>
-  <si>
-    <t>Ha Duc 3</t>
-  </si>
-  <si>
-    <t>Phuoc</t>
-  </si>
-  <si>
-    <t>dphuoc4320001@gmail.com</t>
-  </si>
-  <si>
-    <t>0961622464</t>
-  </si>
-  <si>
-    <t>Thac sĩ</t>
-  </si>
-  <si>
-    <t>dphuoc432000@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Student Code</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,9 +67,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,112 +408,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="8" width="10" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>